<commit_message>
finish intro to pandas
</commit_message>
<xml_diff>
--- a/python/patterns/IntroPandas.xlsx
+++ b/python/patterns/IntroPandas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\python\patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5117B5-74E6-4057-970B-3AF80401AA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A925CA25-4E10-4719-A90D-36155B75891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Question</t>
   </si>
@@ -177,6 +177,36 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/reshape-data-concatenate/solutions/4141091/line-by-line-explanation-easy-solution-beginner-friendly-pandas/?envType=study-plan-v2&amp;envId=introduction-to-pandas&amp;lang=pythondata </t>
+  </si>
+  <si>
+    <t>2889. Reshape Data: Pivot</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reshape-data-pivot/solutions/4141174/pandas-1-line-elegant-short-and-more-pandas-solutions/?envType=study-plan-v2&amp;envId=introduction-to-pandas&amp;lang=pythondata</t>
+  </si>
+  <si>
+    <t>Use df.pivot(index='month', columns='city', values='temperature')</t>
+  </si>
+  <si>
+    <t>2890. Reshape Data: Melt</t>
+  </si>
+  <si>
+    <t>Use pd.melt(report, id_vars=['product'], var_name='quarter', value_name='sales')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/reshape-data-melt/solutions/4141084/line-by-line-explanation-easy-solution-beginner-friendly-pandas/?envType=study-plan-v2&amp;envId=introduction-to-pandas&amp;lang=pythondata </t>
+  </si>
+  <si>
+    <t>Advanced Techniques</t>
+  </si>
+  <si>
+    <t>2891. Method Chaining</t>
+  </si>
+  <si>
+    <t>Chain methods: return animals[animals['weight'] &gt; 100].sort_values(['weight'], ascending=False,)[['name']]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/method-chaining/solutions/4134716/easy-pandas-solution-one-liner-beginner-friendly/ </t>
   </si>
 </sst>
 </file>
@@ -273,8 +303,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E13" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E16" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -549,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
@@ -785,6 +815,57 @@
         <v>46</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{788B1500-00C9-499E-A112-ABFDE08A32E9}"/>
@@ -798,11 +879,14 @@
     <hyperlink ref="E11" r:id="rId9" xr:uid="{31141867-748A-4760-AA0F-33CDEAAC13DA}"/>
     <hyperlink ref="E12" r:id="rId10" xr:uid="{0890EAEE-008E-4212-B6C6-6CD7A990088F}"/>
     <hyperlink ref="E13" r:id="rId11" xr:uid="{EFA8ED04-BF40-4626-A876-AD59292EBA4D}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{B1F31529-D75B-42D4-842D-654BCBCA54C8}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{40775046-78B3-4D5C-9110-BC29A5B398EE}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{EFECB81C-6798-4865-91F2-D538792A5A8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>